<commit_message>
small adjustment to the XML practical
</commit_message>
<xml_diff>
--- a/Practical14/autophagosome.xlsx
+++ b/Practical14/autophagosome.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17426\Desktop\IBI1_2019-20\Practical14\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB619201-1E9A-4744-9C70-91956D4DF603}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -370,12 +364,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -383,15 +377,8 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="宋体"/>
-      <family val="3"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -437,23 +424,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -495,7 +474,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -527,27 +506,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -579,24 +540,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -772,20 +715,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="1" width="18.875" customWidth="1"/>
-    <col min="2" max="2" width="35.125" customWidth="1"/>
-    <col min="3" max="3" width="102.25" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -799,7 +736,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -813,7 +750,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -827,7 +764,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -841,7 +778,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -855,7 +792,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -869,7 +806,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -883,7 +820,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -897,7 +834,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -911,7 +848,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -925,7 +862,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -939,7 +876,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -953,7 +890,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -967,7 +904,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -981,7 +918,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -995,7 +932,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1009,7 +946,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:4">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1023,7 +960,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:4">
       <c r="A18" t="s">
         <v>20</v>
       </c>
@@ -1037,7 +974,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:4">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1051,7 +988,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:4">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1065,7 +1002,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:4">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1079,7 +1016,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:4">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1093,7 +1030,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:4">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1107,7 +1044,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:4">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1121,7 +1058,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:4">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1135,7 +1072,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:4">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1149,7 +1086,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:4">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1163,7 +1100,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:4">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1177,7 +1114,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:4">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1191,7 +1128,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:4">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1205,7 +1142,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:4">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1219,7 +1156,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:4">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1233,7 +1170,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:4">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1247,7 +1184,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:4">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1261,7 +1198,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:4">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1275,7 +1212,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:4">
       <c r="A36" t="s">
         <v>38</v>
       </c>
@@ -1290,8 +1227,6 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>